<commit_message>
Updated skills matrix and added a DevOps column
</commit_message>
<xml_diff>
--- a/skills_matrix.xlsx
+++ b/skills_matrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A0E740-14D5-4012-9C7F-E13E0B7D62D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5C4282-167D-9C46-9401-000ACBDB5F7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Continuous Improvement Toolkit . www.citoolkit.com</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>kumar.sabnis@gmail.com</t>
+  </si>
+  <si>
+    <t>rupakg@gmail.com</t>
+  </si>
+  <si>
+    <t>DevOps</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,65 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="79">
+  <dxfs count="85">
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFCCFFB4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC00CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1703,338 +1767,338 @@
   <dimension ref="A1:P238"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="4" customWidth="1"/>
-    <col min="5" max="13" width="14.81640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="2.81640625" style="4" customWidth="1"/>
-    <col min="16" max="245" width="9.08984375" style="4"/>
+    <col min="1" max="1" width="2.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="4" customWidth="1"/>
+    <col min="5" max="13" width="14.83203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="2.83203125" style="4" customWidth="1"/>
+    <col min="16" max="245" width="9.1640625" style="4"/>
     <col min="246" max="248" width="3" style="4" customWidth="1"/>
-    <col min="249" max="268" width="5.81640625" style="4" customWidth="1"/>
-    <col min="269" max="269" width="13.90625" style="4" customWidth="1"/>
-    <col min="270" max="270" width="19.453125" style="4" customWidth="1"/>
-    <col min="271" max="501" width="9.08984375" style="4"/>
+    <col min="249" max="268" width="5.83203125" style="4" customWidth="1"/>
+    <col min="269" max="269" width="13.83203125" style="4" customWidth="1"/>
+    <col min="270" max="270" width="19.5" style="4" customWidth="1"/>
+    <col min="271" max="501" width="9.1640625" style="4"/>
     <col min="502" max="504" width="3" style="4" customWidth="1"/>
-    <col min="505" max="524" width="5.81640625" style="4" customWidth="1"/>
-    <col min="525" max="525" width="13.90625" style="4" customWidth="1"/>
-    <col min="526" max="526" width="19.453125" style="4" customWidth="1"/>
-    <col min="527" max="757" width="9.08984375" style="4"/>
+    <col min="505" max="524" width="5.83203125" style="4" customWidth="1"/>
+    <col min="525" max="525" width="13.83203125" style="4" customWidth="1"/>
+    <col min="526" max="526" width="19.5" style="4" customWidth="1"/>
+    <col min="527" max="757" width="9.1640625" style="4"/>
     <col min="758" max="760" width="3" style="4" customWidth="1"/>
-    <col min="761" max="780" width="5.81640625" style="4" customWidth="1"/>
-    <col min="781" max="781" width="13.90625" style="4" customWidth="1"/>
-    <col min="782" max="782" width="19.453125" style="4" customWidth="1"/>
-    <col min="783" max="1013" width="9.08984375" style="4"/>
+    <col min="761" max="780" width="5.83203125" style="4" customWidth="1"/>
+    <col min="781" max="781" width="13.83203125" style="4" customWidth="1"/>
+    <col min="782" max="782" width="19.5" style="4" customWidth="1"/>
+    <col min="783" max="1013" width="9.1640625" style="4"/>
     <col min="1014" max="1016" width="3" style="4" customWidth="1"/>
-    <col min="1017" max="1036" width="5.81640625" style="4" customWidth="1"/>
-    <col min="1037" max="1037" width="13.90625" style="4" customWidth="1"/>
-    <col min="1038" max="1038" width="19.453125" style="4" customWidth="1"/>
-    <col min="1039" max="1269" width="9.08984375" style="4"/>
+    <col min="1017" max="1036" width="5.83203125" style="4" customWidth="1"/>
+    <col min="1037" max="1037" width="13.83203125" style="4" customWidth="1"/>
+    <col min="1038" max="1038" width="19.5" style="4" customWidth="1"/>
+    <col min="1039" max="1269" width="9.1640625" style="4"/>
     <col min="1270" max="1272" width="3" style="4" customWidth="1"/>
-    <col min="1273" max="1292" width="5.81640625" style="4" customWidth="1"/>
-    <col min="1293" max="1293" width="13.90625" style="4" customWidth="1"/>
-    <col min="1294" max="1294" width="19.453125" style="4" customWidth="1"/>
-    <col min="1295" max="1525" width="9.08984375" style="4"/>
+    <col min="1273" max="1292" width="5.83203125" style="4" customWidth="1"/>
+    <col min="1293" max="1293" width="13.83203125" style="4" customWidth="1"/>
+    <col min="1294" max="1294" width="19.5" style="4" customWidth="1"/>
+    <col min="1295" max="1525" width="9.1640625" style="4"/>
     <col min="1526" max="1528" width="3" style="4" customWidth="1"/>
-    <col min="1529" max="1548" width="5.81640625" style="4" customWidth="1"/>
-    <col min="1549" max="1549" width="13.90625" style="4" customWidth="1"/>
-    <col min="1550" max="1550" width="19.453125" style="4" customWidth="1"/>
-    <col min="1551" max="1781" width="9.08984375" style="4"/>
+    <col min="1529" max="1548" width="5.83203125" style="4" customWidth="1"/>
+    <col min="1549" max="1549" width="13.83203125" style="4" customWidth="1"/>
+    <col min="1550" max="1550" width="19.5" style="4" customWidth="1"/>
+    <col min="1551" max="1781" width="9.1640625" style="4"/>
     <col min="1782" max="1784" width="3" style="4" customWidth="1"/>
-    <col min="1785" max="1804" width="5.81640625" style="4" customWidth="1"/>
-    <col min="1805" max="1805" width="13.90625" style="4" customWidth="1"/>
-    <col min="1806" max="1806" width="19.453125" style="4" customWidth="1"/>
-    <col min="1807" max="2037" width="9.08984375" style="4"/>
+    <col min="1785" max="1804" width="5.83203125" style="4" customWidth="1"/>
+    <col min="1805" max="1805" width="13.83203125" style="4" customWidth="1"/>
+    <col min="1806" max="1806" width="19.5" style="4" customWidth="1"/>
+    <col min="1807" max="2037" width="9.1640625" style="4"/>
     <col min="2038" max="2040" width="3" style="4" customWidth="1"/>
-    <col min="2041" max="2060" width="5.81640625" style="4" customWidth="1"/>
-    <col min="2061" max="2061" width="13.90625" style="4" customWidth="1"/>
-    <col min="2062" max="2062" width="19.453125" style="4" customWidth="1"/>
-    <col min="2063" max="2293" width="9.08984375" style="4"/>
+    <col min="2041" max="2060" width="5.83203125" style="4" customWidth="1"/>
+    <col min="2061" max="2061" width="13.83203125" style="4" customWidth="1"/>
+    <col min="2062" max="2062" width="19.5" style="4" customWidth="1"/>
+    <col min="2063" max="2293" width="9.1640625" style="4"/>
     <col min="2294" max="2296" width="3" style="4" customWidth="1"/>
-    <col min="2297" max="2316" width="5.81640625" style="4" customWidth="1"/>
-    <col min="2317" max="2317" width="13.90625" style="4" customWidth="1"/>
-    <col min="2318" max="2318" width="19.453125" style="4" customWidth="1"/>
-    <col min="2319" max="2549" width="9.08984375" style="4"/>
+    <col min="2297" max="2316" width="5.83203125" style="4" customWidth="1"/>
+    <col min="2317" max="2317" width="13.83203125" style="4" customWidth="1"/>
+    <col min="2318" max="2318" width="19.5" style="4" customWidth="1"/>
+    <col min="2319" max="2549" width="9.1640625" style="4"/>
     <col min="2550" max="2552" width="3" style="4" customWidth="1"/>
-    <col min="2553" max="2572" width="5.81640625" style="4" customWidth="1"/>
-    <col min="2573" max="2573" width="13.90625" style="4" customWidth="1"/>
-    <col min="2574" max="2574" width="19.453125" style="4" customWidth="1"/>
-    <col min="2575" max="2805" width="9.08984375" style="4"/>
+    <col min="2553" max="2572" width="5.83203125" style="4" customWidth="1"/>
+    <col min="2573" max="2573" width="13.83203125" style="4" customWidth="1"/>
+    <col min="2574" max="2574" width="19.5" style="4" customWidth="1"/>
+    <col min="2575" max="2805" width="9.1640625" style="4"/>
     <col min="2806" max="2808" width="3" style="4" customWidth="1"/>
-    <col min="2809" max="2828" width="5.81640625" style="4" customWidth="1"/>
-    <col min="2829" max="2829" width="13.90625" style="4" customWidth="1"/>
-    <col min="2830" max="2830" width="19.453125" style="4" customWidth="1"/>
-    <col min="2831" max="3061" width="9.08984375" style="4"/>
+    <col min="2809" max="2828" width="5.83203125" style="4" customWidth="1"/>
+    <col min="2829" max="2829" width="13.83203125" style="4" customWidth="1"/>
+    <col min="2830" max="2830" width="19.5" style="4" customWidth="1"/>
+    <col min="2831" max="3061" width="9.1640625" style="4"/>
     <col min="3062" max="3064" width="3" style="4" customWidth="1"/>
-    <col min="3065" max="3084" width="5.81640625" style="4" customWidth="1"/>
-    <col min="3085" max="3085" width="13.90625" style="4" customWidth="1"/>
-    <col min="3086" max="3086" width="19.453125" style="4" customWidth="1"/>
-    <col min="3087" max="3317" width="9.08984375" style="4"/>
+    <col min="3065" max="3084" width="5.83203125" style="4" customWidth="1"/>
+    <col min="3085" max="3085" width="13.83203125" style="4" customWidth="1"/>
+    <col min="3086" max="3086" width="19.5" style="4" customWidth="1"/>
+    <col min="3087" max="3317" width="9.1640625" style="4"/>
     <col min="3318" max="3320" width="3" style="4" customWidth="1"/>
-    <col min="3321" max="3340" width="5.81640625" style="4" customWidth="1"/>
-    <col min="3341" max="3341" width="13.90625" style="4" customWidth="1"/>
-    <col min="3342" max="3342" width="19.453125" style="4" customWidth="1"/>
-    <col min="3343" max="3573" width="9.08984375" style="4"/>
+    <col min="3321" max="3340" width="5.83203125" style="4" customWidth="1"/>
+    <col min="3341" max="3341" width="13.83203125" style="4" customWidth="1"/>
+    <col min="3342" max="3342" width="19.5" style="4" customWidth="1"/>
+    <col min="3343" max="3573" width="9.1640625" style="4"/>
     <col min="3574" max="3576" width="3" style="4" customWidth="1"/>
-    <col min="3577" max="3596" width="5.81640625" style="4" customWidth="1"/>
-    <col min="3597" max="3597" width="13.90625" style="4" customWidth="1"/>
-    <col min="3598" max="3598" width="19.453125" style="4" customWidth="1"/>
-    <col min="3599" max="3829" width="9.08984375" style="4"/>
+    <col min="3577" max="3596" width="5.83203125" style="4" customWidth="1"/>
+    <col min="3597" max="3597" width="13.83203125" style="4" customWidth="1"/>
+    <col min="3598" max="3598" width="19.5" style="4" customWidth="1"/>
+    <col min="3599" max="3829" width="9.1640625" style="4"/>
     <col min="3830" max="3832" width="3" style="4" customWidth="1"/>
-    <col min="3833" max="3852" width="5.81640625" style="4" customWidth="1"/>
-    <col min="3853" max="3853" width="13.90625" style="4" customWidth="1"/>
-    <col min="3854" max="3854" width="19.453125" style="4" customWidth="1"/>
-    <col min="3855" max="4085" width="9.08984375" style="4"/>
+    <col min="3833" max="3852" width="5.83203125" style="4" customWidth="1"/>
+    <col min="3853" max="3853" width="13.83203125" style="4" customWidth="1"/>
+    <col min="3854" max="3854" width="19.5" style="4" customWidth="1"/>
+    <col min="3855" max="4085" width="9.1640625" style="4"/>
     <col min="4086" max="4088" width="3" style="4" customWidth="1"/>
-    <col min="4089" max="4108" width="5.81640625" style="4" customWidth="1"/>
-    <col min="4109" max="4109" width="13.90625" style="4" customWidth="1"/>
-    <col min="4110" max="4110" width="19.453125" style="4" customWidth="1"/>
-    <col min="4111" max="4341" width="9.08984375" style="4"/>
+    <col min="4089" max="4108" width="5.83203125" style="4" customWidth="1"/>
+    <col min="4109" max="4109" width="13.83203125" style="4" customWidth="1"/>
+    <col min="4110" max="4110" width="19.5" style="4" customWidth="1"/>
+    <col min="4111" max="4341" width="9.1640625" style="4"/>
     <col min="4342" max="4344" width="3" style="4" customWidth="1"/>
-    <col min="4345" max="4364" width="5.81640625" style="4" customWidth="1"/>
-    <col min="4365" max="4365" width="13.90625" style="4" customWidth="1"/>
-    <col min="4366" max="4366" width="19.453125" style="4" customWidth="1"/>
-    <col min="4367" max="4597" width="9.08984375" style="4"/>
+    <col min="4345" max="4364" width="5.83203125" style="4" customWidth="1"/>
+    <col min="4365" max="4365" width="13.83203125" style="4" customWidth="1"/>
+    <col min="4366" max="4366" width="19.5" style="4" customWidth="1"/>
+    <col min="4367" max="4597" width="9.1640625" style="4"/>
     <col min="4598" max="4600" width="3" style="4" customWidth="1"/>
-    <col min="4601" max="4620" width="5.81640625" style="4" customWidth="1"/>
-    <col min="4621" max="4621" width="13.90625" style="4" customWidth="1"/>
-    <col min="4622" max="4622" width="19.453125" style="4" customWidth="1"/>
-    <col min="4623" max="4853" width="9.08984375" style="4"/>
+    <col min="4601" max="4620" width="5.83203125" style="4" customWidth="1"/>
+    <col min="4621" max="4621" width="13.83203125" style="4" customWidth="1"/>
+    <col min="4622" max="4622" width="19.5" style="4" customWidth="1"/>
+    <col min="4623" max="4853" width="9.1640625" style="4"/>
     <col min="4854" max="4856" width="3" style="4" customWidth="1"/>
-    <col min="4857" max="4876" width="5.81640625" style="4" customWidth="1"/>
-    <col min="4877" max="4877" width="13.90625" style="4" customWidth="1"/>
-    <col min="4878" max="4878" width="19.453125" style="4" customWidth="1"/>
-    <col min="4879" max="5109" width="9.08984375" style="4"/>
+    <col min="4857" max="4876" width="5.83203125" style="4" customWidth="1"/>
+    <col min="4877" max="4877" width="13.83203125" style="4" customWidth="1"/>
+    <col min="4878" max="4878" width="19.5" style="4" customWidth="1"/>
+    <col min="4879" max="5109" width="9.1640625" style="4"/>
     <col min="5110" max="5112" width="3" style="4" customWidth="1"/>
-    <col min="5113" max="5132" width="5.81640625" style="4" customWidth="1"/>
-    <col min="5133" max="5133" width="13.90625" style="4" customWidth="1"/>
-    <col min="5134" max="5134" width="19.453125" style="4" customWidth="1"/>
-    <col min="5135" max="5365" width="9.08984375" style="4"/>
+    <col min="5113" max="5132" width="5.83203125" style="4" customWidth="1"/>
+    <col min="5133" max="5133" width="13.83203125" style="4" customWidth="1"/>
+    <col min="5134" max="5134" width="19.5" style="4" customWidth="1"/>
+    <col min="5135" max="5365" width="9.1640625" style="4"/>
     <col min="5366" max="5368" width="3" style="4" customWidth="1"/>
-    <col min="5369" max="5388" width="5.81640625" style="4" customWidth="1"/>
-    <col min="5389" max="5389" width="13.90625" style="4" customWidth="1"/>
-    <col min="5390" max="5390" width="19.453125" style="4" customWidth="1"/>
-    <col min="5391" max="5621" width="9.08984375" style="4"/>
+    <col min="5369" max="5388" width="5.83203125" style="4" customWidth="1"/>
+    <col min="5389" max="5389" width="13.83203125" style="4" customWidth="1"/>
+    <col min="5390" max="5390" width="19.5" style="4" customWidth="1"/>
+    <col min="5391" max="5621" width="9.1640625" style="4"/>
     <col min="5622" max="5624" width="3" style="4" customWidth="1"/>
-    <col min="5625" max="5644" width="5.81640625" style="4" customWidth="1"/>
-    <col min="5645" max="5645" width="13.90625" style="4" customWidth="1"/>
-    <col min="5646" max="5646" width="19.453125" style="4" customWidth="1"/>
-    <col min="5647" max="5877" width="9.08984375" style="4"/>
+    <col min="5625" max="5644" width="5.83203125" style="4" customWidth="1"/>
+    <col min="5645" max="5645" width="13.83203125" style="4" customWidth="1"/>
+    <col min="5646" max="5646" width="19.5" style="4" customWidth="1"/>
+    <col min="5647" max="5877" width="9.1640625" style="4"/>
     <col min="5878" max="5880" width="3" style="4" customWidth="1"/>
-    <col min="5881" max="5900" width="5.81640625" style="4" customWidth="1"/>
-    <col min="5901" max="5901" width="13.90625" style="4" customWidth="1"/>
-    <col min="5902" max="5902" width="19.453125" style="4" customWidth="1"/>
-    <col min="5903" max="6133" width="9.08984375" style="4"/>
+    <col min="5881" max="5900" width="5.83203125" style="4" customWidth="1"/>
+    <col min="5901" max="5901" width="13.83203125" style="4" customWidth="1"/>
+    <col min="5902" max="5902" width="19.5" style="4" customWidth="1"/>
+    <col min="5903" max="6133" width="9.1640625" style="4"/>
     <col min="6134" max="6136" width="3" style="4" customWidth="1"/>
-    <col min="6137" max="6156" width="5.81640625" style="4" customWidth="1"/>
-    <col min="6157" max="6157" width="13.90625" style="4" customWidth="1"/>
-    <col min="6158" max="6158" width="19.453125" style="4" customWidth="1"/>
-    <col min="6159" max="6389" width="9.08984375" style="4"/>
+    <col min="6137" max="6156" width="5.83203125" style="4" customWidth="1"/>
+    <col min="6157" max="6157" width="13.83203125" style="4" customWidth="1"/>
+    <col min="6158" max="6158" width="19.5" style="4" customWidth="1"/>
+    <col min="6159" max="6389" width="9.1640625" style="4"/>
     <col min="6390" max="6392" width="3" style="4" customWidth="1"/>
-    <col min="6393" max="6412" width="5.81640625" style="4" customWidth="1"/>
-    <col min="6413" max="6413" width="13.90625" style="4" customWidth="1"/>
-    <col min="6414" max="6414" width="19.453125" style="4" customWidth="1"/>
-    <col min="6415" max="6645" width="9.08984375" style="4"/>
+    <col min="6393" max="6412" width="5.83203125" style="4" customWidth="1"/>
+    <col min="6413" max="6413" width="13.83203125" style="4" customWidth="1"/>
+    <col min="6414" max="6414" width="19.5" style="4" customWidth="1"/>
+    <col min="6415" max="6645" width="9.1640625" style="4"/>
     <col min="6646" max="6648" width="3" style="4" customWidth="1"/>
-    <col min="6649" max="6668" width="5.81640625" style="4" customWidth="1"/>
-    <col min="6669" max="6669" width="13.90625" style="4" customWidth="1"/>
-    <col min="6670" max="6670" width="19.453125" style="4" customWidth="1"/>
-    <col min="6671" max="6901" width="9.08984375" style="4"/>
+    <col min="6649" max="6668" width="5.83203125" style="4" customWidth="1"/>
+    <col min="6669" max="6669" width="13.83203125" style="4" customWidth="1"/>
+    <col min="6670" max="6670" width="19.5" style="4" customWidth="1"/>
+    <col min="6671" max="6901" width="9.1640625" style="4"/>
     <col min="6902" max="6904" width="3" style="4" customWidth="1"/>
-    <col min="6905" max="6924" width="5.81640625" style="4" customWidth="1"/>
-    <col min="6925" max="6925" width="13.90625" style="4" customWidth="1"/>
-    <col min="6926" max="6926" width="19.453125" style="4" customWidth="1"/>
-    <col min="6927" max="7157" width="9.08984375" style="4"/>
+    <col min="6905" max="6924" width="5.83203125" style="4" customWidth="1"/>
+    <col min="6925" max="6925" width="13.83203125" style="4" customWidth="1"/>
+    <col min="6926" max="6926" width="19.5" style="4" customWidth="1"/>
+    <col min="6927" max="7157" width="9.1640625" style="4"/>
     <col min="7158" max="7160" width="3" style="4" customWidth="1"/>
-    <col min="7161" max="7180" width="5.81640625" style="4" customWidth="1"/>
-    <col min="7181" max="7181" width="13.90625" style="4" customWidth="1"/>
-    <col min="7182" max="7182" width="19.453125" style="4" customWidth="1"/>
-    <col min="7183" max="7413" width="9.08984375" style="4"/>
+    <col min="7161" max="7180" width="5.83203125" style="4" customWidth="1"/>
+    <col min="7181" max="7181" width="13.83203125" style="4" customWidth="1"/>
+    <col min="7182" max="7182" width="19.5" style="4" customWidth="1"/>
+    <col min="7183" max="7413" width="9.1640625" style="4"/>
     <col min="7414" max="7416" width="3" style="4" customWidth="1"/>
-    <col min="7417" max="7436" width="5.81640625" style="4" customWidth="1"/>
-    <col min="7437" max="7437" width="13.90625" style="4" customWidth="1"/>
-    <col min="7438" max="7438" width="19.453125" style="4" customWidth="1"/>
-    <col min="7439" max="7669" width="9.08984375" style="4"/>
+    <col min="7417" max="7436" width="5.83203125" style="4" customWidth="1"/>
+    <col min="7437" max="7437" width="13.83203125" style="4" customWidth="1"/>
+    <col min="7438" max="7438" width="19.5" style="4" customWidth="1"/>
+    <col min="7439" max="7669" width="9.1640625" style="4"/>
     <col min="7670" max="7672" width="3" style="4" customWidth="1"/>
-    <col min="7673" max="7692" width="5.81640625" style="4" customWidth="1"/>
-    <col min="7693" max="7693" width="13.90625" style="4" customWidth="1"/>
-    <col min="7694" max="7694" width="19.453125" style="4" customWidth="1"/>
-    <col min="7695" max="7925" width="9.08984375" style="4"/>
+    <col min="7673" max="7692" width="5.83203125" style="4" customWidth="1"/>
+    <col min="7693" max="7693" width="13.83203125" style="4" customWidth="1"/>
+    <col min="7694" max="7694" width="19.5" style="4" customWidth="1"/>
+    <col min="7695" max="7925" width="9.1640625" style="4"/>
     <col min="7926" max="7928" width="3" style="4" customWidth="1"/>
-    <col min="7929" max="7948" width="5.81640625" style="4" customWidth="1"/>
-    <col min="7949" max="7949" width="13.90625" style="4" customWidth="1"/>
-    <col min="7950" max="7950" width="19.453125" style="4" customWidth="1"/>
-    <col min="7951" max="8181" width="9.08984375" style="4"/>
+    <col min="7929" max="7948" width="5.83203125" style="4" customWidth="1"/>
+    <col min="7949" max="7949" width="13.83203125" style="4" customWidth="1"/>
+    <col min="7950" max="7950" width="19.5" style="4" customWidth="1"/>
+    <col min="7951" max="8181" width="9.1640625" style="4"/>
     <col min="8182" max="8184" width="3" style="4" customWidth="1"/>
-    <col min="8185" max="8204" width="5.81640625" style="4" customWidth="1"/>
-    <col min="8205" max="8205" width="13.90625" style="4" customWidth="1"/>
-    <col min="8206" max="8206" width="19.453125" style="4" customWidth="1"/>
-    <col min="8207" max="8437" width="9.08984375" style="4"/>
+    <col min="8185" max="8204" width="5.83203125" style="4" customWidth="1"/>
+    <col min="8205" max="8205" width="13.83203125" style="4" customWidth="1"/>
+    <col min="8206" max="8206" width="19.5" style="4" customWidth="1"/>
+    <col min="8207" max="8437" width="9.1640625" style="4"/>
     <col min="8438" max="8440" width="3" style="4" customWidth="1"/>
-    <col min="8441" max="8460" width="5.81640625" style="4" customWidth="1"/>
-    <col min="8461" max="8461" width="13.90625" style="4" customWidth="1"/>
-    <col min="8462" max="8462" width="19.453125" style="4" customWidth="1"/>
-    <col min="8463" max="8693" width="9.08984375" style="4"/>
+    <col min="8441" max="8460" width="5.83203125" style="4" customWidth="1"/>
+    <col min="8461" max="8461" width="13.83203125" style="4" customWidth="1"/>
+    <col min="8462" max="8462" width="19.5" style="4" customWidth="1"/>
+    <col min="8463" max="8693" width="9.1640625" style="4"/>
     <col min="8694" max="8696" width="3" style="4" customWidth="1"/>
-    <col min="8697" max="8716" width="5.81640625" style="4" customWidth="1"/>
-    <col min="8717" max="8717" width="13.90625" style="4" customWidth="1"/>
-    <col min="8718" max="8718" width="19.453125" style="4" customWidth="1"/>
-    <col min="8719" max="8949" width="9.08984375" style="4"/>
+    <col min="8697" max="8716" width="5.83203125" style="4" customWidth="1"/>
+    <col min="8717" max="8717" width="13.83203125" style="4" customWidth="1"/>
+    <col min="8718" max="8718" width="19.5" style="4" customWidth="1"/>
+    <col min="8719" max="8949" width="9.1640625" style="4"/>
     <col min="8950" max="8952" width="3" style="4" customWidth="1"/>
-    <col min="8953" max="8972" width="5.81640625" style="4" customWidth="1"/>
-    <col min="8973" max="8973" width="13.90625" style="4" customWidth="1"/>
-    <col min="8974" max="8974" width="19.453125" style="4" customWidth="1"/>
-    <col min="8975" max="9205" width="9.08984375" style="4"/>
+    <col min="8953" max="8972" width="5.83203125" style="4" customWidth="1"/>
+    <col min="8973" max="8973" width="13.83203125" style="4" customWidth="1"/>
+    <col min="8974" max="8974" width="19.5" style="4" customWidth="1"/>
+    <col min="8975" max="9205" width="9.1640625" style="4"/>
     <col min="9206" max="9208" width="3" style="4" customWidth="1"/>
-    <col min="9209" max="9228" width="5.81640625" style="4" customWidth="1"/>
-    <col min="9229" max="9229" width="13.90625" style="4" customWidth="1"/>
-    <col min="9230" max="9230" width="19.453125" style="4" customWidth="1"/>
-    <col min="9231" max="9461" width="9.08984375" style="4"/>
+    <col min="9209" max="9228" width="5.83203125" style="4" customWidth="1"/>
+    <col min="9229" max="9229" width="13.83203125" style="4" customWidth="1"/>
+    <col min="9230" max="9230" width="19.5" style="4" customWidth="1"/>
+    <col min="9231" max="9461" width="9.1640625" style="4"/>
     <col min="9462" max="9464" width="3" style="4" customWidth="1"/>
-    <col min="9465" max="9484" width="5.81640625" style="4" customWidth="1"/>
-    <col min="9485" max="9485" width="13.90625" style="4" customWidth="1"/>
-    <col min="9486" max="9486" width="19.453125" style="4" customWidth="1"/>
-    <col min="9487" max="9717" width="9.08984375" style="4"/>
+    <col min="9465" max="9484" width="5.83203125" style="4" customWidth="1"/>
+    <col min="9485" max="9485" width="13.83203125" style="4" customWidth="1"/>
+    <col min="9486" max="9486" width="19.5" style="4" customWidth="1"/>
+    <col min="9487" max="9717" width="9.1640625" style="4"/>
     <col min="9718" max="9720" width="3" style="4" customWidth="1"/>
-    <col min="9721" max="9740" width="5.81640625" style="4" customWidth="1"/>
-    <col min="9741" max="9741" width="13.90625" style="4" customWidth="1"/>
-    <col min="9742" max="9742" width="19.453125" style="4" customWidth="1"/>
-    <col min="9743" max="9973" width="9.08984375" style="4"/>
+    <col min="9721" max="9740" width="5.83203125" style="4" customWidth="1"/>
+    <col min="9741" max="9741" width="13.83203125" style="4" customWidth="1"/>
+    <col min="9742" max="9742" width="19.5" style="4" customWidth="1"/>
+    <col min="9743" max="9973" width="9.1640625" style="4"/>
     <col min="9974" max="9976" width="3" style="4" customWidth="1"/>
-    <col min="9977" max="9996" width="5.81640625" style="4" customWidth="1"/>
-    <col min="9997" max="9997" width="13.90625" style="4" customWidth="1"/>
-    <col min="9998" max="9998" width="19.453125" style="4" customWidth="1"/>
-    <col min="9999" max="10229" width="9.08984375" style="4"/>
+    <col min="9977" max="9996" width="5.83203125" style="4" customWidth="1"/>
+    <col min="9997" max="9997" width="13.83203125" style="4" customWidth="1"/>
+    <col min="9998" max="9998" width="19.5" style="4" customWidth="1"/>
+    <col min="9999" max="10229" width="9.1640625" style="4"/>
     <col min="10230" max="10232" width="3" style="4" customWidth="1"/>
-    <col min="10233" max="10252" width="5.81640625" style="4" customWidth="1"/>
-    <col min="10253" max="10253" width="13.90625" style="4" customWidth="1"/>
-    <col min="10254" max="10254" width="19.453125" style="4" customWidth="1"/>
-    <col min="10255" max="10485" width="9.08984375" style="4"/>
+    <col min="10233" max="10252" width="5.83203125" style="4" customWidth="1"/>
+    <col min="10253" max="10253" width="13.83203125" style="4" customWidth="1"/>
+    <col min="10254" max="10254" width="19.5" style="4" customWidth="1"/>
+    <col min="10255" max="10485" width="9.1640625" style="4"/>
     <col min="10486" max="10488" width="3" style="4" customWidth="1"/>
-    <col min="10489" max="10508" width="5.81640625" style="4" customWidth="1"/>
-    <col min="10509" max="10509" width="13.90625" style="4" customWidth="1"/>
-    <col min="10510" max="10510" width="19.453125" style="4" customWidth="1"/>
-    <col min="10511" max="10741" width="9.08984375" style="4"/>
+    <col min="10489" max="10508" width="5.83203125" style="4" customWidth="1"/>
+    <col min="10509" max="10509" width="13.83203125" style="4" customWidth="1"/>
+    <col min="10510" max="10510" width="19.5" style="4" customWidth="1"/>
+    <col min="10511" max="10741" width="9.1640625" style="4"/>
     <col min="10742" max="10744" width="3" style="4" customWidth="1"/>
-    <col min="10745" max="10764" width="5.81640625" style="4" customWidth="1"/>
-    <col min="10765" max="10765" width="13.90625" style="4" customWidth="1"/>
-    <col min="10766" max="10766" width="19.453125" style="4" customWidth="1"/>
-    <col min="10767" max="10997" width="9.08984375" style="4"/>
+    <col min="10745" max="10764" width="5.83203125" style="4" customWidth="1"/>
+    <col min="10765" max="10765" width="13.83203125" style="4" customWidth="1"/>
+    <col min="10766" max="10766" width="19.5" style="4" customWidth="1"/>
+    <col min="10767" max="10997" width="9.1640625" style="4"/>
     <col min="10998" max="11000" width="3" style="4" customWidth="1"/>
-    <col min="11001" max="11020" width="5.81640625" style="4" customWidth="1"/>
-    <col min="11021" max="11021" width="13.90625" style="4" customWidth="1"/>
-    <col min="11022" max="11022" width="19.453125" style="4" customWidth="1"/>
-    <col min="11023" max="11253" width="9.08984375" style="4"/>
+    <col min="11001" max="11020" width="5.83203125" style="4" customWidth="1"/>
+    <col min="11021" max="11021" width="13.83203125" style="4" customWidth="1"/>
+    <col min="11022" max="11022" width="19.5" style="4" customWidth="1"/>
+    <col min="11023" max="11253" width="9.1640625" style="4"/>
     <col min="11254" max="11256" width="3" style="4" customWidth="1"/>
-    <col min="11257" max="11276" width="5.81640625" style="4" customWidth="1"/>
-    <col min="11277" max="11277" width="13.90625" style="4" customWidth="1"/>
-    <col min="11278" max="11278" width="19.453125" style="4" customWidth="1"/>
-    <col min="11279" max="11509" width="9.08984375" style="4"/>
+    <col min="11257" max="11276" width="5.83203125" style="4" customWidth="1"/>
+    <col min="11277" max="11277" width="13.83203125" style="4" customWidth="1"/>
+    <col min="11278" max="11278" width="19.5" style="4" customWidth="1"/>
+    <col min="11279" max="11509" width="9.1640625" style="4"/>
     <col min="11510" max="11512" width="3" style="4" customWidth="1"/>
-    <col min="11513" max="11532" width="5.81640625" style="4" customWidth="1"/>
-    <col min="11533" max="11533" width="13.90625" style="4" customWidth="1"/>
-    <col min="11534" max="11534" width="19.453125" style="4" customWidth="1"/>
-    <col min="11535" max="11765" width="9.08984375" style="4"/>
+    <col min="11513" max="11532" width="5.83203125" style="4" customWidth="1"/>
+    <col min="11533" max="11533" width="13.83203125" style="4" customWidth="1"/>
+    <col min="11534" max="11534" width="19.5" style="4" customWidth="1"/>
+    <col min="11535" max="11765" width="9.1640625" style="4"/>
     <col min="11766" max="11768" width="3" style="4" customWidth="1"/>
-    <col min="11769" max="11788" width="5.81640625" style="4" customWidth="1"/>
-    <col min="11789" max="11789" width="13.90625" style="4" customWidth="1"/>
-    <col min="11790" max="11790" width="19.453125" style="4" customWidth="1"/>
-    <col min="11791" max="12021" width="9.08984375" style="4"/>
+    <col min="11769" max="11788" width="5.83203125" style="4" customWidth="1"/>
+    <col min="11789" max="11789" width="13.83203125" style="4" customWidth="1"/>
+    <col min="11790" max="11790" width="19.5" style="4" customWidth="1"/>
+    <col min="11791" max="12021" width="9.1640625" style="4"/>
     <col min="12022" max="12024" width="3" style="4" customWidth="1"/>
-    <col min="12025" max="12044" width="5.81640625" style="4" customWidth="1"/>
-    <col min="12045" max="12045" width="13.90625" style="4" customWidth="1"/>
-    <col min="12046" max="12046" width="19.453125" style="4" customWidth="1"/>
-    <col min="12047" max="12277" width="9.08984375" style="4"/>
+    <col min="12025" max="12044" width="5.83203125" style="4" customWidth="1"/>
+    <col min="12045" max="12045" width="13.83203125" style="4" customWidth="1"/>
+    <col min="12046" max="12046" width="19.5" style="4" customWidth="1"/>
+    <col min="12047" max="12277" width="9.1640625" style="4"/>
     <col min="12278" max="12280" width="3" style="4" customWidth="1"/>
-    <col min="12281" max="12300" width="5.81640625" style="4" customWidth="1"/>
-    <col min="12301" max="12301" width="13.90625" style="4" customWidth="1"/>
-    <col min="12302" max="12302" width="19.453125" style="4" customWidth="1"/>
-    <col min="12303" max="12533" width="9.08984375" style="4"/>
+    <col min="12281" max="12300" width="5.83203125" style="4" customWidth="1"/>
+    <col min="12301" max="12301" width="13.83203125" style="4" customWidth="1"/>
+    <col min="12302" max="12302" width="19.5" style="4" customWidth="1"/>
+    <col min="12303" max="12533" width="9.1640625" style="4"/>
     <col min="12534" max="12536" width="3" style="4" customWidth="1"/>
-    <col min="12537" max="12556" width="5.81640625" style="4" customWidth="1"/>
-    <col min="12557" max="12557" width="13.90625" style="4" customWidth="1"/>
-    <col min="12558" max="12558" width="19.453125" style="4" customWidth="1"/>
-    <col min="12559" max="12789" width="9.08984375" style="4"/>
+    <col min="12537" max="12556" width="5.83203125" style="4" customWidth="1"/>
+    <col min="12557" max="12557" width="13.83203125" style="4" customWidth="1"/>
+    <col min="12558" max="12558" width="19.5" style="4" customWidth="1"/>
+    <col min="12559" max="12789" width="9.1640625" style="4"/>
     <col min="12790" max="12792" width="3" style="4" customWidth="1"/>
-    <col min="12793" max="12812" width="5.81640625" style="4" customWidth="1"/>
-    <col min="12813" max="12813" width="13.90625" style="4" customWidth="1"/>
-    <col min="12814" max="12814" width="19.453125" style="4" customWidth="1"/>
-    <col min="12815" max="13045" width="9.08984375" style="4"/>
+    <col min="12793" max="12812" width="5.83203125" style="4" customWidth="1"/>
+    <col min="12813" max="12813" width="13.83203125" style="4" customWidth="1"/>
+    <col min="12814" max="12814" width="19.5" style="4" customWidth="1"/>
+    <col min="12815" max="13045" width="9.1640625" style="4"/>
     <col min="13046" max="13048" width="3" style="4" customWidth="1"/>
-    <col min="13049" max="13068" width="5.81640625" style="4" customWidth="1"/>
-    <col min="13069" max="13069" width="13.90625" style="4" customWidth="1"/>
-    <col min="13070" max="13070" width="19.453125" style="4" customWidth="1"/>
-    <col min="13071" max="13301" width="9.08984375" style="4"/>
+    <col min="13049" max="13068" width="5.83203125" style="4" customWidth="1"/>
+    <col min="13069" max="13069" width="13.83203125" style="4" customWidth="1"/>
+    <col min="13070" max="13070" width="19.5" style="4" customWidth="1"/>
+    <col min="13071" max="13301" width="9.1640625" style="4"/>
     <col min="13302" max="13304" width="3" style="4" customWidth="1"/>
-    <col min="13305" max="13324" width="5.81640625" style="4" customWidth="1"/>
-    <col min="13325" max="13325" width="13.90625" style="4" customWidth="1"/>
-    <col min="13326" max="13326" width="19.453125" style="4" customWidth="1"/>
-    <col min="13327" max="13557" width="9.08984375" style="4"/>
+    <col min="13305" max="13324" width="5.83203125" style="4" customWidth="1"/>
+    <col min="13325" max="13325" width="13.83203125" style="4" customWidth="1"/>
+    <col min="13326" max="13326" width="19.5" style="4" customWidth="1"/>
+    <col min="13327" max="13557" width="9.1640625" style="4"/>
     <col min="13558" max="13560" width="3" style="4" customWidth="1"/>
-    <col min="13561" max="13580" width="5.81640625" style="4" customWidth="1"/>
-    <col min="13581" max="13581" width="13.90625" style="4" customWidth="1"/>
-    <col min="13582" max="13582" width="19.453125" style="4" customWidth="1"/>
-    <col min="13583" max="13813" width="9.08984375" style="4"/>
+    <col min="13561" max="13580" width="5.83203125" style="4" customWidth="1"/>
+    <col min="13581" max="13581" width="13.83203125" style="4" customWidth="1"/>
+    <col min="13582" max="13582" width="19.5" style="4" customWidth="1"/>
+    <col min="13583" max="13813" width="9.1640625" style="4"/>
     <col min="13814" max="13816" width="3" style="4" customWidth="1"/>
-    <col min="13817" max="13836" width="5.81640625" style="4" customWidth="1"/>
-    <col min="13837" max="13837" width="13.90625" style="4" customWidth="1"/>
-    <col min="13838" max="13838" width="19.453125" style="4" customWidth="1"/>
-    <col min="13839" max="14069" width="9.08984375" style="4"/>
+    <col min="13817" max="13836" width="5.83203125" style="4" customWidth="1"/>
+    <col min="13837" max="13837" width="13.83203125" style="4" customWidth="1"/>
+    <col min="13838" max="13838" width="19.5" style="4" customWidth="1"/>
+    <col min="13839" max="14069" width="9.1640625" style="4"/>
     <col min="14070" max="14072" width="3" style="4" customWidth="1"/>
-    <col min="14073" max="14092" width="5.81640625" style="4" customWidth="1"/>
-    <col min="14093" max="14093" width="13.90625" style="4" customWidth="1"/>
-    <col min="14094" max="14094" width="19.453125" style="4" customWidth="1"/>
-    <col min="14095" max="14325" width="9.08984375" style="4"/>
+    <col min="14073" max="14092" width="5.83203125" style="4" customWidth="1"/>
+    <col min="14093" max="14093" width="13.83203125" style="4" customWidth="1"/>
+    <col min="14094" max="14094" width="19.5" style="4" customWidth="1"/>
+    <col min="14095" max="14325" width="9.1640625" style="4"/>
     <col min="14326" max="14328" width="3" style="4" customWidth="1"/>
-    <col min="14329" max="14348" width="5.81640625" style="4" customWidth="1"/>
-    <col min="14349" max="14349" width="13.90625" style="4" customWidth="1"/>
-    <col min="14350" max="14350" width="19.453125" style="4" customWidth="1"/>
-    <col min="14351" max="14581" width="9.08984375" style="4"/>
+    <col min="14329" max="14348" width="5.83203125" style="4" customWidth="1"/>
+    <col min="14349" max="14349" width="13.83203125" style="4" customWidth="1"/>
+    <col min="14350" max="14350" width="19.5" style="4" customWidth="1"/>
+    <col min="14351" max="14581" width="9.1640625" style="4"/>
     <col min="14582" max="14584" width="3" style="4" customWidth="1"/>
-    <col min="14585" max="14604" width="5.81640625" style="4" customWidth="1"/>
-    <col min="14605" max="14605" width="13.90625" style="4" customWidth="1"/>
-    <col min="14606" max="14606" width="19.453125" style="4" customWidth="1"/>
-    <col min="14607" max="14837" width="9.08984375" style="4"/>
+    <col min="14585" max="14604" width="5.83203125" style="4" customWidth="1"/>
+    <col min="14605" max="14605" width="13.83203125" style="4" customWidth="1"/>
+    <col min="14606" max="14606" width="19.5" style="4" customWidth="1"/>
+    <col min="14607" max="14837" width="9.1640625" style="4"/>
     <col min="14838" max="14840" width="3" style="4" customWidth="1"/>
-    <col min="14841" max="14860" width="5.81640625" style="4" customWidth="1"/>
-    <col min="14861" max="14861" width="13.90625" style="4" customWidth="1"/>
-    <col min="14862" max="14862" width="19.453125" style="4" customWidth="1"/>
-    <col min="14863" max="15093" width="9.08984375" style="4"/>
+    <col min="14841" max="14860" width="5.83203125" style="4" customWidth="1"/>
+    <col min="14861" max="14861" width="13.83203125" style="4" customWidth="1"/>
+    <col min="14862" max="14862" width="19.5" style="4" customWidth="1"/>
+    <col min="14863" max="15093" width="9.1640625" style="4"/>
     <col min="15094" max="15096" width="3" style="4" customWidth="1"/>
-    <col min="15097" max="15116" width="5.81640625" style="4" customWidth="1"/>
-    <col min="15117" max="15117" width="13.90625" style="4" customWidth="1"/>
-    <col min="15118" max="15118" width="19.453125" style="4" customWidth="1"/>
-    <col min="15119" max="15349" width="9.08984375" style="4"/>
+    <col min="15097" max="15116" width="5.83203125" style="4" customWidth="1"/>
+    <col min="15117" max="15117" width="13.83203125" style="4" customWidth="1"/>
+    <col min="15118" max="15118" width="19.5" style="4" customWidth="1"/>
+    <col min="15119" max="15349" width="9.1640625" style="4"/>
     <col min="15350" max="15352" width="3" style="4" customWidth="1"/>
-    <col min="15353" max="15372" width="5.81640625" style="4" customWidth="1"/>
-    <col min="15373" max="15373" width="13.90625" style="4" customWidth="1"/>
-    <col min="15374" max="15374" width="19.453125" style="4" customWidth="1"/>
-    <col min="15375" max="15605" width="9.08984375" style="4"/>
+    <col min="15353" max="15372" width="5.83203125" style="4" customWidth="1"/>
+    <col min="15373" max="15373" width="13.83203125" style="4" customWidth="1"/>
+    <col min="15374" max="15374" width="19.5" style="4" customWidth="1"/>
+    <col min="15375" max="15605" width="9.1640625" style="4"/>
     <col min="15606" max="15608" width="3" style="4" customWidth="1"/>
-    <col min="15609" max="15628" width="5.81640625" style="4" customWidth="1"/>
-    <col min="15629" max="15629" width="13.90625" style="4" customWidth="1"/>
-    <col min="15630" max="15630" width="19.453125" style="4" customWidth="1"/>
-    <col min="15631" max="15861" width="9.08984375" style="4"/>
+    <col min="15609" max="15628" width="5.83203125" style="4" customWidth="1"/>
+    <col min="15629" max="15629" width="13.83203125" style="4" customWidth="1"/>
+    <col min="15630" max="15630" width="19.5" style="4" customWidth="1"/>
+    <col min="15631" max="15861" width="9.1640625" style="4"/>
     <col min="15862" max="15864" width="3" style="4" customWidth="1"/>
-    <col min="15865" max="15884" width="5.81640625" style="4" customWidth="1"/>
-    <col min="15885" max="15885" width="13.90625" style="4" customWidth="1"/>
-    <col min="15886" max="15886" width="19.453125" style="4" customWidth="1"/>
-    <col min="15887" max="16117" width="9.08984375" style="4"/>
+    <col min="15865" max="15884" width="5.83203125" style="4" customWidth="1"/>
+    <col min="15885" max="15885" width="13.83203125" style="4" customWidth="1"/>
+    <col min="15886" max="15886" width="19.5" style="4" customWidth="1"/>
+    <col min="15887" max="16117" width="9.1640625" style="4"/>
     <col min="16118" max="16120" width="3" style="4" customWidth="1"/>
-    <col min="16121" max="16140" width="5.81640625" style="4" customWidth="1"/>
-    <col min="16141" max="16141" width="13.90625" style="4" customWidth="1"/>
-    <col min="16142" max="16142" width="19.453125" style="4" customWidth="1"/>
-    <col min="16143" max="16147" width="9.08984375" style="4"/>
-    <col min="16148" max="16384" width="8.90625" style="4"/>
+    <col min="16121" max="16140" width="5.83203125" style="4" customWidth="1"/>
+    <col min="16141" max="16141" width="13.83203125" style="4" customWidth="1"/>
+    <col min="16142" max="16142" width="19.5" style="4" customWidth="1"/>
+    <col min="16143" max="16147" width="9.1640625" style="4"/>
+    <col min="16148" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="31" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="48" t="s">
         <v>22</v>
@@ -2057,7 +2121,7 @@
       </c>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -2081,7 +2145,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2184,7 @@
       </c>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
@@ -2146,7 +2210,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:16" s="6" customFormat="1" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="6" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2165,7 +2229,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16" s="18" customFormat="1" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" s="18" customFormat="1" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -2181,7 +2245,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="17"/>
     </row>
-    <row r="7" spans="1:16" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7" s="42" t="s">
         <v>5</v>
@@ -2210,7 +2274,9 @@
       <c r="J7" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="39" t="s">
+        <v>46</v>
+      </c>
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
       <c r="N7" s="44" t="s">
@@ -2218,7 +2284,7 @@
       </c>
       <c r="O7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="21">
         <v>1</v>
       </c>
@@ -2258,7 +2324,7 @@
       </c>
       <c r="O8" s="28"/>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="21">
         <v>2</v>
       </c>
@@ -2298,7 +2364,7 @@
       </c>
       <c r="O9" s="28"/>
     </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="21">
         <v>3</v>
       </c>
@@ -2338,29 +2404,49 @@
       </c>
       <c r="O10" s="28"/>
     </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="21">
         <v>4</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
+      <c r="B11" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="40">
+        <v>2</v>
+      </c>
+      <c r="F11" s="40">
+        <v>3</v>
+      </c>
+      <c r="G11" s="40">
+        <v>2</v>
+      </c>
+      <c r="H11" s="40">
+        <v>3</v>
+      </c>
+      <c r="I11" s="40">
+        <v>2</v>
+      </c>
+      <c r="J11" s="40">
+        <v>3</v>
+      </c>
+      <c r="K11" s="40">
+        <v>4</v>
+      </c>
       <c r="L11" s="40"/>
       <c r="M11" s="40"/>
-      <c r="N11" s="47" t="str">
+      <c r="N11" s="47">
         <f t="shared" si="0"/>
-        <v/>
+        <v>19</v>
       </c>
       <c r="O11" s="28"/>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="21">
         <v>5</v>
       </c>
@@ -2382,7 +2468,7 @@
       </c>
       <c r="O12" s="28"/>
     </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="21">
         <v>6</v>
       </c>
@@ -2404,7 +2490,7 @@
       </c>
       <c r="O13" s="28"/>
     </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="21">
         <v>7</v>
       </c>
@@ -2426,7 +2512,7 @@
       </c>
       <c r="O14" s="28"/>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="21">
         <v>8</v>
       </c>
@@ -2448,7 +2534,7 @@
       </c>
       <c r="O15" s="28"/>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="21">
         <v>9</v>
       </c>
@@ -2470,7 +2556,7 @@
       </c>
       <c r="O16" s="28"/>
     </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="21">
         <v>10</v>
       </c>
@@ -2492,7 +2578,7 @@
       </c>
       <c r="O17" s="28"/>
     </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="21">
         <v>11</v>
       </c>
@@ -2514,7 +2600,7 @@
       </c>
       <c r="O18" s="28"/>
     </row>
-    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="21">
         <v>12</v>
       </c>
@@ -2536,7 +2622,7 @@
       </c>
       <c r="O19" s="28"/>
     </row>
-    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="21">
         <v>13</v>
       </c>
@@ -2558,7 +2644,7 @@
       </c>
       <c r="O20" s="28"/>
     </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="21">
         <v>14</v>
       </c>
@@ -2580,7 +2666,7 @@
       </c>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -2589,31 +2675,31 @@
       </c>
       <c r="E22" s="45">
         <f t="shared" ref="E22:J22" si="1">IF(AND(SUM(E8:E21)=0,COUNT(E8:E21)=0),"",SUM(E8:E21))</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F22" s="45">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G22" s="45">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H22" s="45">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I22" s="45">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J22" s="45">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="K22" s="45" t="str">
+        <v>9</v>
+      </c>
+      <c r="K22" s="45">
         <f>IF(AND(SUM(K8:K21)=0,COUNT(K8:K21)=0),"",SUM(K8:K21))</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="L22" s="45" t="str">
         <f t="shared" ref="L22" si="2">IF(AND(SUM(L8:L21)=0,COUNT(L8:L21)=0),"",SUM(L8:L21))</f>
@@ -2626,7 +2712,7 @@
       <c r="N22" s="46"/>
       <c r="O22" s="29"/>
     </row>
-    <row r="23" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="21"/>
       <c r="B23" s="30"/>
       <c r="C23" s="31" t="s">
@@ -2659,9 +2745,9 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K23" s="41" t="str">
+      <c r="K23" s="41">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="L23" s="41" t="str">
         <f t="shared" si="4"/>
@@ -2674,7 +2760,7 @@
       <c r="N23" s="46"/>
       <c r="O23" s="29"/>
     </row>
-    <row r="24" spans="1:15" s="18" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="18" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -2690,8 +2776,8 @@
       <c r="M24" s="24"/>
       <c r="N24" s="25"/>
     </row>
-    <row r="25" spans="1:15" s="18" customFormat="1" ht="14.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:15" s="18" customFormat="1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="18" customFormat="1" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:15" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="B26" s="52" t="s">
         <v>0</v>
       </c>
@@ -2708,49 +2794,49 @@
       <c r="M26" s="52"/>
       <c r="N26" s="52"/>
     </row>
-    <row r="27" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="2:14" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -2765,7 +2851,7 @@
       <c r="M45" s="18"/>
       <c r="N45" s="18"/>
     </row>
-    <row r="46" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2780,7 +2866,7 @@
       <c r="M46" s="18"/>
       <c r="N46" s="18"/>
     </row>
-    <row r="47" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -2795,7 +2881,7 @@
       <c r="M47" s="18"/>
       <c r="N47" s="18"/>
     </row>
-    <row r="48" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -2810,7 +2896,7 @@
       <c r="M48" s="18"/>
       <c r="N48" s="18"/>
     </row>
-    <row r="49" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -2825,7 +2911,7 @@
       <c r="M49" s="18"/>
       <c r="N49" s="18"/>
     </row>
-    <row r="50" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -2840,7 +2926,7 @@
       <c r="M50" s="18"/>
       <c r="N50" s="18"/>
     </row>
-    <row r="51" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -2855,7 +2941,7 @@
       <c r="M51" s="18"/>
       <c r="N51" s="18"/>
     </row>
-    <row r="52" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -2870,7 +2956,7 @@
       <c r="M52" s="18"/>
       <c r="N52" s="18"/>
     </row>
-    <row r="53" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -2885,7 +2971,7 @@
       <c r="M53" s="18"/>
       <c r="N53" s="18"/>
     </row>
-    <row r="54" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -2900,7 +2986,7 @@
       <c r="M54" s="18"/>
       <c r="N54" s="18"/>
     </row>
-    <row r="55" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2915,7 +3001,7 @@
       <c r="M55" s="18"/>
       <c r="N55" s="18"/>
     </row>
-    <row r="56" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -2930,7 +3016,7 @@
       <c r="M56" s="18"/>
       <c r="N56" s="18"/>
     </row>
-    <row r="57" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
@@ -2945,7 +3031,7 @@
       <c r="M57" s="18"/>
       <c r="N57" s="18"/>
     </row>
-    <row r="58" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -2960,7 +3046,7 @@
       <c r="M58" s="18"/>
       <c r="N58" s="18"/>
     </row>
-    <row r="59" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -2975,7 +3061,7 @@
       <c r="M59" s="18"/>
       <c r="N59" s="18"/>
     </row>
-    <row r="60" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -2990,7 +3076,7 @@
       <c r="M60" s="18"/>
       <c r="N60" s="18"/>
     </row>
-    <row r="61" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -3005,7 +3091,7 @@
       <c r="M61" s="18"/>
       <c r="N61" s="18"/>
     </row>
-    <row r="62" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -3020,408 +3106,408 @@
       <c r="M62" s="18"/>
       <c r="N62" s="18"/>
     </row>
-    <row r="63" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="150" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="151" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="152" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="153" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="154" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="155" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="156" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="157" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="158" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="159" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="160" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="161" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="162" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="163" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="164" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="165" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="166" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="167" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="168" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="169" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="171" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="188" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="189" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="190" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="191" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="192" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="193" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="194" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="195" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="196" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="197" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="198" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="199" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="200" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="201" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="202" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="203" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="204" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="205" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="206" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="207" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="208" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="209" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="210" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="211" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="212" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="213" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="214" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="215" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="216" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="217" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="218" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="219" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="220" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="221" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="222" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="223" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="224" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="225" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="226" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="227" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="228" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="229" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="230" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="231" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="232" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="233" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="234" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="235" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="236" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="237" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="238" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="64" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="65" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="66" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="67" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="68" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="69" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="70" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="71" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="72" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="73" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="74" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="75" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="76" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="77" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="78" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="79" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="80" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="81" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="82" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="83" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="84" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="85" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="86" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="87" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="88" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="89" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="90" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="91" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="92" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="93" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="94" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="95" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="96" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="97" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="98" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="99" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="100" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="101" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="102" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="103" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="104" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="105" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="106" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="107" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="108" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="109" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="110" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="111" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="112" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="113" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="114" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="115" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="116" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="117" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="118" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="119" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="120" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="121" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="122" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="123" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="124" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="125" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="126" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="127" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="128" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="129" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="130" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="131" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="132" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="133" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="134" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="135" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="136" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="137" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="138" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="139" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="140" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="141" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="142" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="143" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="144" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="145" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="146" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="147" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="148" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="149" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="150" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="151" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="152" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="153" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="154" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="155" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="156" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="157" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="158" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="159" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="160" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="161" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="162" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="163" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="164" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="165" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="166" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="167" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="168" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="169" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="170" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="171" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="172" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="173" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="174" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="175" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="176" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="177" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="178" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="179" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="180" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="181" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="182" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="183" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="184" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="185" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="186" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="187" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="188" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="189" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="190" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="191" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="192" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="193" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="194" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="195" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="196" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="197" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="198" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="199" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="200" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="201" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="202" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="203" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="204" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="205" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="206" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="207" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="208" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="209" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="210" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="211" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="212" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="213" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="214" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="215" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="216" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="217" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="218" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="219" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="220" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="221" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="222" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="223" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="224" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="225" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="226" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="227" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="228" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="229" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="230" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="231" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="232" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="233" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="234" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="235" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="236" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="237" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="238" s="18" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B26:N26"/>
   </mergeCells>
   <conditionalFormatting sqref="N23 E22:N22">
-    <cfRule type="expression" dxfId="78" priority="536">
+    <cfRule type="expression" dxfId="84" priority="542">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="537">
+    <cfRule type="expression" dxfId="83" priority="543">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="538">
+    <cfRule type="expression" dxfId="82" priority="544">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="539">
+    <cfRule type="expression" dxfId="81" priority="545">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="540">
+    <cfRule type="expression" dxfId="80" priority="546">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="541">
+    <cfRule type="expression" dxfId="79" priority="547">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B20">
-    <cfRule type="expression" dxfId="72" priority="44">
+    <cfRule type="expression" dxfId="78" priority="50">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="45">
+    <cfRule type="expression" dxfId="77" priority="51">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="46">
+    <cfRule type="expression" dxfId="76" priority="52">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="47">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="48">
+    <cfRule type="expression" dxfId="74" priority="54">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="49">
+    <cfRule type="expression" dxfId="73" priority="55">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C20">
-    <cfRule type="expression" dxfId="66" priority="50">
+    <cfRule type="expression" dxfId="72" priority="56">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="51">
+    <cfRule type="expression" dxfId="71" priority="57">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="52">
+    <cfRule type="expression" dxfId="70" priority="58">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="53">
+    <cfRule type="expression" dxfId="69" priority="59">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="54">
+    <cfRule type="expression" dxfId="68" priority="60">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="55">
+    <cfRule type="expression" dxfId="67" priority="61">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D20">
-    <cfRule type="expression" dxfId="60" priority="56">
+    <cfRule type="expression" dxfId="66" priority="62">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="57">
+    <cfRule type="expression" dxfId="65" priority="63">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="58">
+    <cfRule type="expression" dxfId="64" priority="64">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="63" priority="65">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="60">
+    <cfRule type="expression" dxfId="62" priority="66">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="61">
+    <cfRule type="expression" dxfId="61" priority="67">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="54" priority="68">
+    <cfRule type="expression" dxfId="60" priority="74">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="69">
+    <cfRule type="expression" dxfId="59" priority="75">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="70">
+    <cfRule type="expression" dxfId="58" priority="76">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="71">
+    <cfRule type="expression" dxfId="57" priority="77">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="72">
+    <cfRule type="expression" dxfId="56" priority="78">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="73">
+    <cfRule type="expression" dxfId="55" priority="79">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="48" priority="74">
+    <cfRule type="expression" dxfId="54" priority="80">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="75">
+    <cfRule type="expression" dxfId="53" priority="81">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="76">
+    <cfRule type="expression" dxfId="52" priority="82">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="77">
+    <cfRule type="expression" dxfId="51" priority="83">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="78">
+    <cfRule type="expression" dxfId="50" priority="84">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="79">
+    <cfRule type="expression" dxfId="49" priority="85">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="42" priority="80">
+    <cfRule type="expression" dxfId="48" priority="86">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="81">
+    <cfRule type="expression" dxfId="47" priority="87">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="82">
+    <cfRule type="expression" dxfId="46" priority="88">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="83">
+    <cfRule type="expression" dxfId="45" priority="89">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="84">
+    <cfRule type="expression" dxfId="44" priority="90">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="85">
+    <cfRule type="expression" dxfId="43" priority="91">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:B23">
-    <cfRule type="expression" dxfId="36" priority="116">
+    <cfRule type="expression" dxfId="42" priority="122">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="117">
+    <cfRule type="expression" dxfId="41" priority="123">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="118">
+    <cfRule type="expression" dxfId="40" priority="124">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="119">
+    <cfRule type="expression" dxfId="39" priority="125">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="120">
+    <cfRule type="expression" dxfId="38" priority="126">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="121">
+    <cfRule type="expression" dxfId="37" priority="127">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="expression" dxfId="30" priority="122">
+    <cfRule type="expression" dxfId="36" priority="128">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="123">
+    <cfRule type="expression" dxfId="35" priority="129">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="124">
+    <cfRule type="expression" dxfId="34" priority="130">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="125">
+    <cfRule type="expression" dxfId="33" priority="131">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="126">
+    <cfRule type="expression" dxfId="32" priority="132">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="127">
+    <cfRule type="expression" dxfId="31" priority="133">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:D23">
-    <cfRule type="expression" dxfId="24" priority="128">
+    <cfRule type="expression" dxfId="30" priority="134">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="129">
+    <cfRule type="expression" dxfId="29" priority="135">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="130">
+    <cfRule type="expression" dxfId="28" priority="136">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="131">
+    <cfRule type="expression" dxfId="27" priority="137">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="132">
+    <cfRule type="expression" dxfId="26" priority="138">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="133">
+    <cfRule type="expression" dxfId="25" priority="139">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23 E22:N22">
-    <cfRule type="expression" dxfId="18" priority="134">
+    <cfRule type="expression" dxfId="24" priority="140">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="135">
+    <cfRule type="expression" dxfId="23" priority="141">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="136">
+    <cfRule type="expression" dxfId="22" priority="142">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="137">
+    <cfRule type="expression" dxfId="21" priority="143">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="138">
+    <cfRule type="expression" dxfId="20" priority="144">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="139">
+    <cfRule type="expression" dxfId="19" priority="145">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N21">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3431,27 +3517,27 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>#REF!="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>#REF!="99% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="16">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>#REF!="75% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="17">
+    <cfRule type="expression" dxfId="15" priority="23">
       <formula>#REF!="50% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="14" priority="24">
       <formula>#REF!="25% or less"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="19">
+    <cfRule type="expression" dxfId="13" priority="25">
       <formula>#REF!="Not started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:M22">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3462,33 +3548,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:M3 E8:M21">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="I3:M3 E12:M21 E8:J11 L8:M11">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>$N$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>$M$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="545" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="551" operator="equal">
       <formula>$J$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="548" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="554" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:M23">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
       <formula>$B$23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:M1">
-    <cfRule type="iconSet" priority="1">
+    <cfRule type="iconSet" priority="7">
       <iconSet iconSet="5Quarters" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3496,6 +3582,26 @@
         <cfvo type="percent" val="60"/>
         <cfvo type="percent" val="80"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:K11">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>$N$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>$M$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>$L$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>$K$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>$J$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3507,9 +3613,10 @@
     <hyperlink ref="C8" r:id="rId1" xr:uid="{8E267587-2336-4D11-98B7-B3907FCC5FAB}"/>
     <hyperlink ref="C9" r:id="rId2" xr:uid="{94781757-CF5D-40BD-AEBA-24F99C5F6486}"/>
     <hyperlink ref="C10" r:id="rId3" xr:uid="{751ADA5E-CDF5-4B8A-92D5-A403194A3517}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{7E640C12-D54F-B449-A94C-F78A25BAE2C0}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.27559055118110237" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="7.874015748031496E-2" footer="7.874015748031496E-2"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="4294967293" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>